<commit_message>
Modificaciones realizar para dar soporte a ficheros de museos
</commit_message>
<xml_diff>
--- a/data/formatted/Datos WCAG Ayuntamientos_formatted.xlsx
+++ b/data/formatted/Datos WCAG Ayuntamientos_formatted.xlsx
@@ -5801,7 +5801,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">1.3.6 Identify Purpose </t>
+          <t>1.3.6 Identify Purpose</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">1.4.12 Text Spacing </t>
+          <t>1.4.12 Text Spacing</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -13052,7 +13052,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">2.2.6 Timeouts </t>
+          <t>2.2.6 Timeouts</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -25580,7 +25580,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">4.1.3 Status Messages </t>
+          <t>4.1.3 Status Messages</t>
         </is>
       </c>
       <c r="D96" t="n">

</xml_diff>